<commit_message>
Leva em consideração o periodo de duração das disciplinas para fazer os agrupamentos
</commit_message>
<xml_diff>
--- a/dados/horarios_2024_1.xlsx
+++ b/dados/horarios_2024_1.xlsx
@@ -21,91 +21,88 @@
     <style:font-face style:name="Noto Sans CJK SC" svg:font-family="'Noto Sans CJK SC'" style:font-family-generic="system" style:font-pitch="variable"/>
   </office:font-face-decls>
   <office:automatic-styles>
+    <style:style style:name="co1" style:family="table-column">
+      <style:table-column-properties fo:break-before="auto" style:column-width="2.258cm"/>
+    </style:style>
     <style:style style:name="co2" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="1.559cm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="24.996cm"/>
     </style:style>
     <style:style style:name="co3" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="11.845cm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="1.369cm"/>
     </style:style>
     <style:style style:name="co4" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="1.369cm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="7.089cm"/>
     </style:style>
     <style:style style:name="co5" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="7.089cm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="2.268cm"/>
     </style:style>
     <style:style style:name="co6" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="2.268cm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="32.478cm"/>
     </style:style>
     <style:style style:name="co7" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="11.947cm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="14.194cm"/>
     </style:style>
     <style:style style:name="co8" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="14.194cm"/>
-    </style:style>
-    <style:style style:name="co10" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="4.752cm"/>
     </style:style>
-    <style:style style:name="co9" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="2.258cm"/>
+    <style:style style:name="ro1" style:family="table-row">
+      <style:table-row-properties style:row-height="0.452cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+    </style:style>
+    <style:style style:name="ro2" style:family="table-row">
+      <style:table-row-properties style:row-height="0.841cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+    </style:style>
+    <style:style style:name="ro3" style:family="table-row">
+      <style:table-row-properties style:row-height="0.885cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+    </style:style>
+    <style:style style:name="ro4" style:family="table-row">
+      <style:table-row-properties style:row-height="1.058cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
+    </style:style>
+    <style:style style:name="ro5" style:family="table-row">
+      <style:table-row-properties style:row-height="0.919cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ro6" style:family="table-row">
-      <style:table-row-properties style:row-height="0.452cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="1.03cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ro7" style:family="table-row">
-      <style:table-row-properties style:row-height="0.452cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="0.863cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
-    <style:style style:name="ro3" style:family="table-row">
-      <style:table-row-properties style:row-height="0.841cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+    <style:style style:name="ro8" style:family="table-row">
+      <style:table-row-properties style:row-height="1.002cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
-    <style:style style:name="ro4" style:family="table-row">
+    <style:style style:name="ro9" style:family="table-row">
       <style:table-row-properties style:row-height="1.236cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
-    <style:style style:name="ro8" style:family="table-row">
-      <style:table-row-properties style:row-height="1.058cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
-    </style:style>
-    <style:style style:name="ro9" style:family="table-row">
-      <style:table-row-properties style:row-height="0.919cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
-    </style:style>
     <style:style style:name="ro10" style:family="table-row">
-      <style:table-row-properties style:row-height="1.03cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
-    </style:style>
-    <style:style style:name="ro12" style:family="table-row">
-      <style:table-row-properties style:row-height="0.863cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
-    </style:style>
-    <style:style style:name="ro13" style:family="table-row">
-      <style:table-row-properties style:row-height="1.002cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
-    </style:style>
-    <style:style style:name="ro14" style:family="table-row">
       <style:table-row-properties style:row-height="1.753cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ro11" style:family="table-row">
       <style:table-row-properties style:row-height="1.632cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
-    <style:style style:name="ro15" style:family="table-row">
+    <style:style style:name="ro12" style:family="table-row">
       <style:table-row-properties style:row-height="0.45cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
-    <style:style style:name="ro16" style:family="table-row">
+    <style:style style:name="ro13" style:family="table-row">
       <style:table-row-properties style:row-height="1.503cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
-    <style:style style:name="ro17" style:family="table-row">
+    <style:style style:name="ro14" style:family="table-row">
       <style:table-row-properties style:row-height="1.335cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
-    <style:style style:name="ro18" style:family="table-row">
+    <style:style style:name="ro15" style:family="table-row">
       <style:table-row-properties style:row-height="1.309cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
-    <style:style style:name="ro19" style:family="table-row">
+    <style:style style:name="ro16" style:family="table-row">
       <style:table-row-properties style:row-height="1.224cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
-    <style:style style:name="ro20" style:family="table-row">
+    <style:style style:name="ro17" style:family="table-row">
       <style:table-row-properties style:row-height="3.605cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
-    <style:style style:name="ro22" style:family="table-row">
+    <style:style style:name="ro18" style:family="table-row">
       <style:table-row-properties style:row-height="4.001cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
-    <style:style style:name="ro23" style:family="table-row">
+    <style:style style:name="ro19" style:family="table-row">
       <style:table-row-properties style:row-height="2.027cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
-    <style:style style:name="ro24" style:family="table-row">
+    <style:style style:name="ro20" style:family="table-row">
       <style:table-row-properties style:row-height="2.868cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ro21" style:family="table-row">
@@ -113,50 +110,6 @@
     </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
-    </style:style>
-    <style:style style:name="ce11" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="transparent" fo:wrap-option="wrap"/>
-      <style:text-properties fo:font-weight="normal" style:font-weight-asian="normal" style:font-weight-complex="normal"/>
-    </style:style>
-    <style:style style:name="ce15" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="transparent"/>
-      <style:text-properties fo:font-weight="normal" style:font-weight-asian="normal" style:font-weight-complex="normal"/>
-    </style:style>
-    <style:style style:name="ce18" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="transparent" fo:wrap-option="wrap"/>
-    </style:style>
-    <style:style style:name="ce19" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="transparent"/>
-    </style:style>
-    <style:style style:name="ce23" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:wrap-option="wrap"/>
-      <style:text-properties fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
-    </style:style>
-    <style:style style:name="ce24" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:wrap-option="wrap"/>
-    </style:style>
-    <style:style style:name="ce25" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" style:vertical-align="middle"/>
-      <style:paragraph-properties fo:text-align="center"/>
-    </style:style>
-    <style:style style:name="ce26" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:background-color="transparent" fo:wrap-option="no-wrap" style:vertical-align="middle"/>
-      <style:paragraph-properties fo:text-align="center"/>
-    </style:style>
-    <style:style style:name="ce27" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="transparent" fo:wrap-option="no-wrap"/>
-    </style:style>
-    <style:style style:name="ce28" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:background-color="transparent" fo:wrap-option="wrap" style:vertical-align="middle"/>
-      <style:paragraph-properties fo:text-align="center"/>
-    </style:style>
-    <style:style style:name="ce33" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="transparent" fo:wrap-option="wrap"/>
-      <style:text-properties fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
-    </style:style>
-    <style:style style:name="ce34" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="transparent"/>
-      <style:text-properties fo:font-weight="bold" style:font-weight-asian="bold" style:font-weight-complex="bold"/>
     </style:style>
     <style:style style:name="ce14" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="transparent" fo:wrap-option="wrap"/>
@@ -208,6 +161,7 @@
       <table:calculation-settings table:automatic-find-labels="false" table:use-regular-expressions="false" table:use-wildcards="true"/>
       <table:table table:name="_WITH_docentes_por_turma_AS_SELECT_dt_id_turma_COALESCE_COUNT_p__202402211025" table:style-name="ta1">
         <office:forms form:automatic-focus="false" form:apply-design-mode="false"/>
+        <table:table-column table:style-name="co1" table:default-cell-style-name="ce16"/>
         <table:table-column table:style-name="co2" table:default-cell-style-name="ce16"/>
         <table:table-column table:style-name="co3" table:default-cell-style-name="ce16"/>
         <table:table-column table:style-name="co4" table:default-cell-style-name="ce16"/>
@@ -215,10 +169,9 @@
         <table:table-column table:style-name="co6" table:default-cell-style-name="ce16"/>
         <table:table-column table:style-name="co7" table:default-cell-style-name="ce16"/>
         <table:table-column table:style-name="co8" table:default-cell-style-name="ce16"/>
-        <table:table-column table:style-name="co10" table:default-cell-style-name="ce16"/>
-        <table:table-column table:style-name="co9" table:number-columns-repeated="1008" table:default-cell-style-name="ce16"/>
-        <table:table-column table:style-name="co9" table:number-columns-repeated="8" table:default-cell-style-name="ce17"/>
-        <table:table-row table:style-name="ro6">
+        <table:table-column table:style-name="co1" table:number-columns-repeated="1008" table:default-cell-style-name="ce16"/>
+        <table:table-column table:style-name="co1" table:number-columns-repeated="8" table:default-cell-style-name="ce17"/>
+        <table:table-row table:style-name="ro1">
           <table:table-cell table:style-name="ce14" office:value-type="string" calcext:value-type="string">
             <text:p>cod</text:p>
           </table:table-cell>
@@ -243,7 +196,7 @@
           <table:table-cell table:style-name="ce14" table:number-columns-repeated="1009"/>
           <table:table-cell table:style-name="ce20" table:number-columns-repeated="8"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS555</text:p>
           </table:table-cell>
@@ -267,7 +220,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS556</text:p>
           </table:table-cell>
@@ -291,7 +244,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS561</text:p>
           </table:table-cell>
@@ -315,7 +268,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS560</text:p>
           </table:table-cell>
@@ -339,7 +292,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS563</text:p>
           </table:table-cell>
@@ -363,7 +316,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS525</text:p>
           </table:table-cell>
@@ -387,7 +340,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH290</text:p>
           </table:table-cell>
@@ -411,7 +364,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS534</text:p>
           </table:table-cell>
@@ -435,7 +388,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX212</text:p>
           </table:table-cell>
@@ -459,7 +412,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA104</text:p>
           </table:table-cell>
@@ -483,7 +436,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS526</text:p>
           </table:table-cell>
@@ -507,7 +460,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH293</text:p>
           </table:table-cell>
@@ -531,7 +484,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX094</text:p>
           </table:table-cell>
@@ -555,7 +508,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS238</text:p>
           </table:table-cell>
@@ -579,7 +532,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS527</text:p>
           </table:table-cell>
@@ -603,7 +556,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH087</text:p>
           </table:table-cell>
@@ -627,7 +580,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS530</text:p>
           </table:table-cell>
@@ -651,7 +604,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS528</text:p>
           </table:table-cell>
@@ -675,7 +628,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX210</text:p>
           </table:table-cell>
@@ -699,7 +652,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS529</text:p>
           </table:table-cell>
@@ -723,7 +676,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS531</text:p>
           </table:table-cell>
@@ -747,7 +700,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS066</text:p>
           </table:table-cell>
@@ -771,7 +724,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS068</text:p>
           </table:table-cell>
@@ -795,7 +748,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS535</text:p>
           </table:table-cell>
@@ -819,7 +772,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS532</text:p>
           </table:table-cell>
@@ -843,7 +796,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS533</text:p>
           </table:table-cell>
@@ -867,7 +820,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS539</text:p>
           </table:table-cell>
@@ -891,7 +844,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS540</text:p>
           </table:table-cell>
@@ -915,7 +868,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS538</text:p>
           </table:table-cell>
@@ -939,7 +892,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS536</text:p>
           </table:table-cell>
@@ -963,7 +916,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS537</text:p>
           </table:table-cell>
@@ -987,7 +940,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS072</text:p>
           </table:table-cell>
@@ -1011,7 +964,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS542</text:p>
           </table:table-cell>
@@ -1035,7 +988,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS541</text:p>
           </table:table-cell>
@@ -1059,7 +1012,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS081</text:p>
           </table:table-cell>
@@ -1083,7 +1036,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS239</text:p>
           </table:table-cell>
@@ -1107,7 +1060,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS080</text:p>
           </table:table-cell>
@@ -1131,7 +1084,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS077</text:p>
           </table:table-cell>
@@ -1155,7 +1108,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS545</text:p>
           </table:table-cell>
@@ -1179,7 +1132,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS544</text:p>
           </table:table-cell>
@@ -1203,7 +1156,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS235</text:p>
           </table:table-cell>
@@ -1227,7 +1180,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS547</text:p>
           </table:table-cell>
@@ -1253,7 +1206,7 @@
           <table:table-cell table:style-name="ce17" table:number-columns-repeated="1008"/>
           <table:table-cell table:number-columns-repeated="8"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS546</text:p>
           </table:table-cell>
@@ -1277,7 +1230,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS082</text:p>
           </table:table-cell>
@@ -1303,7 +1256,7 @@
           <table:table-cell table:style-name="ce17" table:number-columns-repeated="1008"/>
           <table:table-cell table:number-columns-repeated="8"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS548</text:p>
           </table:table-cell>
@@ -1327,7 +1280,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS549</text:p>
           </table:table-cell>
@@ -1351,7 +1304,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS550</text:p>
           </table:table-cell>
@@ -1375,7 +1328,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS573</text:p>
           </table:table-cell>
@@ -1399,7 +1352,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS551</text:p>
           </table:table-cell>
@@ -1423,7 +1376,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA646</text:p>
           </table:table-cell>
@@ -1447,7 +1400,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA657</text:p>
           </table:table-cell>
@@ -1471,7 +1424,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA653</text:p>
           </table:table-cell>
@@ -1495,7 +1448,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA647</text:p>
           </table:table-cell>
@@ -1519,7 +1472,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA316</text:p>
           </table:table-cell>
@@ -1543,7 +1496,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN190</text:p>
           </table:table-cell>
@@ -1567,7 +1520,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA428</text:p>
           </table:table-cell>
@@ -1591,7 +1544,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA589</text:p>
           </table:table-cell>
@@ -1615,7 +1568,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB0603</text:p>
           </table:table-cell>
@@ -1639,7 +1592,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA0679</text:p>
           </table:table-cell>
@@ -1663,7 +1616,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB0601</text:p>
           </table:table-cell>
@@ -1687,7 +1640,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX1053</text:p>
           </table:table-cell>
@@ -1711,7 +1664,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB0602</text:p>
           </table:table-cell>
@@ -1729,14 +1682,14 @@
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>6M34 (04/03/2024 - 13/07/2024)</text:p>
-            <text:p>6M35 (04/03/2024 – 13/07/2024)</text:p>
+            <text:p>6M35 (04/03/2024 - 13/07/2024)</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="float" office:value="75" calcext:value-type="float">
             <text:p>75</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA0689</text:p>
           </table:table-cell>
@@ -1762,7 +1715,7 @@
           <table:table-cell table:style-name="ce17" table:number-columns-repeated="1008"/>
           <table:table-cell table:number-columns-repeated="8"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX1104</text:p>
           </table:table-cell>
@@ -1779,8 +1732,7 @@
             <text:p>1</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>3M45 4M23 (04/03/2024 - 06/07/2024), 3M4 4M2 (08/07/2024 - 13/07/2024)</text:p>
-            <text:p>34M45 (04/03/2024 - 06/07/2024), 34M4 (08/07/2024 - 13/07/2024)</text:p>
+            <text:p>3M45 4M23 (04/03/2024 - 06/07/2024), 3M4 4M2 (08/07/2024 - 13/07/2024), 34M45 (04/03/2024 - 06/07/2024), 34M4 (08/07/2024 - 13/07/2024)</text:p>
             <text:p/>
           </table:table-cell>
           <table:table-cell office:value-type="float" office:value="75" calcext:value-type="float">
@@ -1788,7 +1740,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB0606</text:p>
           </table:table-cell>
@@ -1812,7 +1764,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX087</text:p>
           </table:table-cell>
@@ -1836,7 +1788,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA0684</text:p>
           </table:table-cell>
@@ -1860,7 +1812,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA0686</text:p>
           </table:table-cell>
@@ -1884,7 +1836,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS0687</text:p>
           </table:table-cell>
@@ -1908,7 +1860,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB057</text:p>
           </table:table-cell>
@@ -1932,7 +1884,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX1047</text:p>
           </table:table-cell>
@@ -1956,7 +1908,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA0685</text:p>
           </table:table-cell>
@@ -1980,7 +1932,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB0607</text:p>
           </table:table-cell>
@@ -2004,7 +1956,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB0608</text:p>
           </table:table-cell>
@@ -2028,7 +1980,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA0683</text:p>
           </table:table-cell>
@@ -2052,7 +2004,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA0683</text:p>
           </table:table-cell>
@@ -2076,7 +2028,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB058</text:p>
           </table:table-cell>
@@ -2100,7 +2052,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA238</text:p>
           </table:table-cell>
@@ -2124,7 +2076,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA038</text:p>
           </table:table-cell>
@@ -2148,7 +2100,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB140</text:p>
           </table:table-cell>
@@ -2172,7 +2124,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB052</text:p>
           </table:table-cell>
@@ -2196,7 +2148,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA039</text:p>
           </table:table-cell>
@@ -2220,7 +2172,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN081</text:p>
           </table:table-cell>
@@ -2244,7 +2196,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA231</text:p>
           </table:table-cell>
@@ -2268,7 +2220,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA225</text:p>
           </table:table-cell>
@@ -2292,7 +2244,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro8">
+        <table:table-row table:style-name="ro4">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA041</text:p>
           </table:table-cell>
@@ -2316,7 +2268,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro9">
+        <table:table-row table:style-name="ro5">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS091</text:p>
           </table:table-cell>
@@ -2340,7 +2292,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA244</text:p>
           </table:table-cell>
@@ -2364,7 +2316,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS247</text:p>
           </table:table-cell>
@@ -2388,7 +2340,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN090</text:p>
           </table:table-cell>
@@ -2412,7 +2364,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA252</text:p>
           </table:table-cell>
@@ -2436,7 +2388,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA287</text:p>
           </table:table-cell>
@@ -2460,7 +2412,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA060</text:p>
           </table:table-cell>
@@ -2484,7 +2436,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA057</text:p>
           </table:table-cell>
@@ -2508,7 +2460,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA259</text:p>
           </table:table-cell>
@@ -2532,7 +2484,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS085</text:p>
           </table:table-cell>
@@ -2556,7 +2508,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA061</text:p>
           </table:table-cell>
@@ -2580,7 +2532,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA268</text:p>
           </table:table-cell>
@@ -2604,7 +2556,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro10">
+        <table:table-row table:style-name="ro6">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA282</text:p>
           </table:table-cell>
@@ -2632,7 +2584,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro12">
+        <table:table-row table:style-name="ro7">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA283</text:p>
           </table:table-cell>
@@ -2662,7 +2614,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro12">
+        <table:table-row table:style-name="ro7">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX1087</text:p>
           </table:table-cell>
@@ -2690,7 +2642,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro9">
+        <table:table-row table:style-name="ro5">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX003</text:p>
           </table:table-cell>
@@ -2718,7 +2670,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX003</text:p>
           </table:table-cell>
@@ -2746,7 +2698,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX210</text:p>
           </table:table-cell>
@@ -2774,7 +2726,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX208</text:p>
           </table:table-cell>
@@ -2802,7 +2754,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX208</text:p>
           </table:table-cell>
@@ -2830,7 +2782,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH293</text:p>
           </table:table-cell>
@@ -2858,7 +2810,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX213</text:p>
           </table:table-cell>
@@ -2886,7 +2838,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX178</text:p>
           </table:table-cell>
@@ -2910,7 +2862,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN253</text:p>
           </table:table-cell>
@@ -2934,7 +2886,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX605</text:p>
           </table:table-cell>
@@ -2958,7 +2910,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX605</text:p>
           </table:table-cell>
@@ -2982,7 +2934,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX055</text:p>
           </table:table-cell>
@@ -3006,7 +2958,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA104</text:p>
           </table:table-cell>
@@ -3030,7 +2982,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX392</text:p>
           </table:table-cell>
@@ -3058,7 +3010,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX608</text:p>
           </table:table-cell>
@@ -3082,7 +3034,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX609</text:p>
           </table:table-cell>
@@ -3110,7 +3062,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX609</text:p>
           </table:table-cell>
@@ -3138,7 +3090,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX098</text:p>
           </table:table-cell>
@@ -3166,7 +3118,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX098</text:p>
           </table:table-cell>
@@ -3194,7 +3146,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX090</text:p>
           </table:table-cell>
@@ -3218,7 +3170,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX615</text:p>
           </table:table-cell>
@@ -3242,7 +3194,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX195</text:p>
           </table:table-cell>
@@ -3266,7 +3218,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX612</text:p>
           </table:table-cell>
@@ -3290,7 +3242,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX613</text:p>
           </table:table-cell>
@@ -3314,7 +3266,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX613</text:p>
           </table:table-cell>
@@ -3338,7 +3290,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX607</text:p>
           </table:table-cell>
@@ -3366,7 +3318,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX091</text:p>
           </table:table-cell>
@@ -3394,7 +3346,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX616</text:p>
           </table:table-cell>
@@ -3422,7 +3374,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX101</text:p>
           </table:table-cell>
@@ -3450,7 +3402,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX110</text:p>
           </table:table-cell>
@@ -3478,7 +3430,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX108</text:p>
           </table:table-cell>
@@ -3502,7 +3454,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN254</text:p>
           </table:table-cell>
@@ -3527,7 +3479,7 @@
           <table:table-cell table:style-name="ce17"/>
           <table:table-cell table:number-columns-repeated="1016"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH290</text:p>
           </table:table-cell>
@@ -3551,7 +3503,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS580</text:p>
           </table:table-cell>
@@ -3575,7 +3527,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX105</text:p>
           </table:table-cell>
@@ -3599,7 +3551,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro13">
+        <table:table-row table:style-name="ro8">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX395</text:p>
           </table:table-cell>
@@ -3623,7 +3575,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX107</text:p>
           </table:table-cell>
@@ -3647,7 +3599,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX618</text:p>
           </table:table-cell>
@@ -3671,7 +3623,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX617</text:p>
           </table:table-cell>
@@ -3699,7 +3651,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS238</text:p>
           </table:table-cell>
@@ -3727,7 +3679,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS239</text:p>
           </table:table-cell>
@@ -3752,7 +3704,7 @@
           <table:table-cell table:style-name="ce17"/>
           <table:table-cell table:number-columns-repeated="1016"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH292</text:p>
           </table:table-cell>
@@ -3776,7 +3728,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX614</text:p>
           </table:table-cell>
@@ -3800,7 +3752,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX638</text:p>
           </table:table-cell>
@@ -3828,7 +3780,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX657</text:p>
           </table:table-cell>
@@ -3856,7 +3808,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX658</text:p>
           </table:table-cell>
@@ -3884,7 +3836,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1433</text:p>
           </table:table-cell>
@@ -3908,7 +3860,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1448</text:p>
           </table:table-cell>
@@ -3932,7 +3884,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1389</text:p>
           </table:table-cell>
@@ -3956,7 +3908,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1390</text:p>
           </table:table-cell>
@@ -3980,7 +3932,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH290</text:p>
           </table:table-cell>
@@ -4004,7 +3956,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH293</text:p>
           </table:table-cell>
@@ -4028,7 +3980,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH291</text:p>
           </table:table-cell>
@@ -4052,7 +4004,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1392</text:p>
           </table:table-cell>
@@ -4076,7 +4028,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1393</text:p>
           </table:table-cell>
@@ -4100,7 +4052,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH839</text:p>
           </table:table-cell>
@@ -4124,7 +4076,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA103</text:p>
           </table:table-cell>
@@ -4148,7 +4100,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1391</text:p>
           </table:table-cell>
@@ -4172,7 +4124,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1399</text:p>
           </table:table-cell>
@@ -4196,7 +4148,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1400</text:p>
           </table:table-cell>
@@ -4220,7 +4172,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX210</text:p>
           </table:table-cell>
@@ -4244,7 +4196,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1401</text:p>
           </table:table-cell>
@@ -4268,7 +4220,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1398</text:p>
           </table:table-cell>
@@ -4292,7 +4244,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH837</text:p>
           </table:table-cell>
@@ -4320,7 +4272,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1407</text:p>
           </table:table-cell>
@@ -4344,7 +4296,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH840</text:p>
           </table:table-cell>
@@ -4368,7 +4320,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro14">
+        <table:table-row table:style-name="ro10">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1408</text:p>
           </table:table-cell>
@@ -4392,7 +4344,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1412</text:p>
           </table:table-cell>
@@ -4422,7 +4374,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA0305</text:p>
           </table:table-cell>
@@ -4446,7 +4398,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA0309</text:p>
           </table:table-cell>
@@ -4476,7 +4428,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA0306</text:p>
           </table:table-cell>
@@ -4504,7 +4456,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA0308</text:p>
           </table:table-cell>
@@ -4532,7 +4484,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA0307</text:p>
           </table:table-cell>
@@ -4560,7 +4512,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH029</text:p>
           </table:table-cell>
@@ -4584,7 +4536,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA001</text:p>
           </table:table-cell>
@@ -4608,7 +4560,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS010</text:p>
           </table:table-cell>
@@ -4632,7 +4584,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS011</text:p>
           </table:table-cell>
@@ -4656,7 +4608,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA020</text:p>
           </table:table-cell>
@@ -4680,7 +4632,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA019</text:p>
           </table:table-cell>
@@ -4710,7 +4662,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB080</text:p>
           </table:table-cell>
@@ -4734,7 +4686,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA018</text:p>
           </table:table-cell>
@@ -4762,7 +4714,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH090</text:p>
           </table:table-cell>
@@ -4786,7 +4738,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH090</text:p>
           </table:table-cell>
@@ -4810,7 +4762,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA045</text:p>
           </table:table-cell>
@@ -4834,7 +4786,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA022</text:p>
           </table:table-cell>
@@ -4860,7 +4812,7 @@
               <text:s/>
               2356T123456 (13/05/2024 - 18/05/2024), 34M2345 
               <text:s/>
-              235T123456 6T12345 (20/05/2024 – 25/05/2024)
+              235T123456 6T12345 (20/05/2024 - 25/05/2024)
             </text:p>
           </table:table-cell>
           <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
@@ -4868,7 +4820,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA046</text:p>
           </table:table-cell>
@@ -4898,7 +4850,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA048</text:p>
           </table:table-cell>
@@ -4922,7 +4874,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX1110</text:p>
           </table:table-cell>
@@ -4946,7 +4898,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX1111</text:p>
           </table:table-cell>
@@ -4970,7 +4922,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX221</text:p>
           </table:table-cell>
@@ -4994,7 +4946,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN191</text:p>
           </table:table-cell>
@@ -5018,7 +4970,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN192</text:p>
           </table:table-cell>
@@ -5042,7 +4994,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN193</text:p>
           </table:table-cell>
@@ -5066,7 +5018,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN198</text:p>
           </table:table-cell>
@@ -5090,7 +5042,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN199</text:p>
           </table:table-cell>
@@ -5114,7 +5066,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN200</text:p>
           </table:table-cell>
@@ -5138,7 +5090,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN203</text:p>
           </table:table-cell>
@@ -5162,7 +5114,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN205</text:p>
           </table:table-cell>
@@ -5186,7 +5138,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX195</text:p>
           </table:table-cell>
@@ -5210,7 +5162,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH292</text:p>
           </table:table-cell>
@@ -5234,7 +5186,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN159</text:p>
           </table:table-cell>
@@ -5258,7 +5210,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX213</text:p>
           </table:table-cell>
@@ -5282,7 +5234,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX294</text:p>
           </table:table-cell>
@@ -5306,7 +5258,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS225</text:p>
           </table:table-cell>
@@ -5330,7 +5282,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB023</text:p>
           </table:table-cell>
@@ -5354,7 +5306,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX399</text:p>
           </table:table-cell>
@@ -5378,7 +5330,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX400</text:p>
           </table:table-cell>
@@ -5402,7 +5354,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN092</text:p>
           </table:table-cell>
@@ -5426,7 +5378,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX462</text:p>
           </table:table-cell>
@@ -5450,7 +5402,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX209</text:p>
           </table:table-cell>
@@ -5474,7 +5426,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN099</text:p>
           </table:table-cell>
@@ -5498,7 +5450,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN100</text:p>
           </table:table-cell>
@@ -5522,7 +5474,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN102</text:p>
           </table:table-cell>
@@ -5546,7 +5498,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH310</text:p>
           </table:table-cell>
@@ -5570,7 +5522,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH309</text:p>
           </table:table-cell>
@@ -5594,7 +5546,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN101</text:p>
           </table:table-cell>
@@ -5618,7 +5570,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN107</text:p>
           </table:table-cell>
@@ -5646,7 +5598,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN105</text:p>
           </table:table-cell>
@@ -5670,7 +5622,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN108</text:p>
           </table:table-cell>
@@ -5740,7 +5692,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN106</text:p>
           </table:table-cell>
@@ -5764,7 +5716,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS238</text:p>
           </table:table-cell>
@@ -5792,7 +5744,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN029</text:p>
           </table:table-cell>
@@ -5820,7 +5772,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS255</text:p>
           </table:table-cell>
@@ -5844,7 +5796,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN117</text:p>
           </table:table-cell>
@@ -5868,7 +5820,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN086</text:p>
           </table:table-cell>
@@ -5892,7 +5844,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN114</text:p>
           </table:table-cell>
@@ -5916,7 +5868,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN113</text:p>
           </table:table-cell>
@@ -5940,7 +5892,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN115</text:p>
           </table:table-cell>
@@ -5964,7 +5916,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN116</text:p>
           </table:table-cell>
@@ -5988,7 +5940,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro15">
+        <table:table-row table:style-name="ro12">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN112</text:p>
           </table:table-cell>
@@ -6012,7 +5964,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN119</text:p>
           </table:table-cell>
@@ -6050,7 +6002,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN118</text:p>
           </table:table-cell>
@@ -6084,7 +6036,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH872</text:p>
           </table:table-cell>
@@ -6108,7 +6060,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH892</text:p>
           </table:table-cell>
@@ -6132,7 +6084,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH823</text:p>
           </table:table-cell>
@@ -6156,7 +6108,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH290</text:p>
           </table:table-cell>
@@ -6180,7 +6132,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH293</text:p>
           </table:table-cell>
@@ -6204,7 +6156,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH822</text:p>
           </table:table-cell>
@@ -6228,7 +6180,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH855</text:p>
           </table:table-cell>
@@ -6252,7 +6204,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH849</text:p>
           </table:table-cell>
@@ -6276,7 +6228,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH846</text:p>
           </table:table-cell>
@@ -6300,7 +6252,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX208</text:p>
           </table:table-cell>
@@ -6324,7 +6276,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS239</text:p>
           </table:table-cell>
@@ -6348,7 +6300,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH851</text:p>
           </table:table-cell>
@@ -6372,7 +6324,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA213</text:p>
           </table:table-cell>
@@ -6396,7 +6348,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1031</text:p>
           </table:table-cell>
@@ -6420,7 +6372,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH291</text:p>
           </table:table-cell>
@@ -6444,7 +6396,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH645</text:p>
           </table:table-cell>
@@ -6468,7 +6420,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH619</text:p>
           </table:table-cell>
@@ -6492,7 +6444,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX555</text:p>
           </table:table-cell>
@@ -6524,7 +6476,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX212</text:p>
           </table:table-cell>
@@ -6548,7 +6500,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA104</text:p>
           </table:table-cell>
@@ -6572,7 +6524,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH621</text:p>
           </table:table-cell>
@@ -6606,7 +6558,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX560</text:p>
           </table:table-cell>
@@ -6638,7 +6590,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA108</text:p>
           </table:table-cell>
@@ -6662,7 +6614,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH630</text:p>
           </table:table-cell>
@@ -6686,7 +6638,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH637</text:p>
           </table:table-cell>
@@ -6710,7 +6662,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH465</text:p>
           </table:table-cell>
@@ -6734,7 +6686,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH468</text:p>
           </table:table-cell>
@@ -6758,7 +6710,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH364</text:p>
           </table:table-cell>
@@ -6782,7 +6734,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX210</text:p>
           </table:table-cell>
@@ -6806,7 +6758,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH363</text:p>
           </table:table-cell>
@@ -6830,7 +6782,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH362</text:p>
           </table:table-cell>
@@ -6854,7 +6806,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA104</text:p>
           </table:table-cell>
@@ -6878,7 +6830,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH370</text:p>
           </table:table-cell>
@@ -6902,7 +6854,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH292</text:p>
           </table:table-cell>
@@ -6926,7 +6878,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH369</text:p>
           </table:table-cell>
@@ -6950,7 +6902,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH293</text:p>
           </table:table-cell>
@@ -6974,7 +6926,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH368</text:p>
           </table:table-cell>
@@ -6998,7 +6950,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH379</text:p>
           </table:table-cell>
@@ -7022,7 +6974,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH378</text:p>
           </table:table-cell>
@@ -7046,7 +6998,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH377</text:p>
           </table:table-cell>
@@ -7070,7 +7022,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH376</text:p>
           </table:table-cell>
@@ -7094,7 +7046,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH375</text:p>
           </table:table-cell>
@@ -7118,7 +7070,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH380</text:p>
           </table:table-cell>
@@ -7142,7 +7094,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH386</text:p>
           </table:table-cell>
@@ -7166,7 +7118,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH385</text:p>
           </table:table-cell>
@@ -7190,7 +7142,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH384</text:p>
           </table:table-cell>
@@ -7214,7 +7166,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH393</text:p>
           </table:table-cell>
@@ -7234,7 +7186,7 @@
             <text:p>
               7M12345 (04/03/2024 - 20/04/2024), 7M123456 
               <text:s/>
-              7N1234 (03/05/2024 – 13/07/2024)
+              7N1234 (03/05/2024 - 13/07/2024)
             </text:p>
           </table:table-cell>
           <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
@@ -7242,7 +7194,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH391</text:p>
           </table:table-cell>
@@ -7266,7 +7218,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH392</text:p>
           </table:table-cell>
@@ -7290,7 +7242,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA469</text:p>
           </table:table-cell>
@@ -7318,7 +7270,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA490</text:p>
           </table:table-cell>
@@ -7346,7 +7298,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA500</text:p>
           </table:table-cell>
@@ -7376,7 +7328,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA506</text:p>
           </table:table-cell>
@@ -7406,7 +7358,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA517</text:p>
           </table:table-cell>
@@ -7434,7 +7386,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA550</text:p>
           </table:table-cell>
@@ -7462,7 +7414,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA553</text:p>
           </table:table-cell>
@@ -7490,7 +7442,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA355</text:p>
           </table:table-cell>
@@ -7514,7 +7466,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH292</text:p>
           </table:table-cell>
@@ -7538,7 +7490,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX002</text:p>
           </table:table-cell>
@@ -7562,7 +7514,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA356</text:p>
           </table:table-cell>
@@ -7586,7 +7538,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA357</text:p>
           </table:table-cell>
@@ -7610,7 +7562,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA001</text:p>
           </table:table-cell>
@@ -7634,7 +7586,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA001</text:p>
           </table:table-cell>
@@ -7658,7 +7610,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA104</text:p>
           </table:table-cell>
@@ -7682,7 +7634,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH011</text:p>
           </table:table-cell>
@@ -7706,7 +7658,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA358</text:p>
           </table:table-cell>
@@ -7736,7 +7688,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX210</text:p>
           </table:table-cell>
@@ -7760,7 +7712,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA363</text:p>
           </table:table-cell>
@@ -7784,7 +7736,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA361</text:p>
           </table:table-cell>
@@ -7814,7 +7766,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro16">
+        <table:table-row table:style-name="ro13">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH029</text:p>
           </table:table-cell>
@@ -7838,7 +7790,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH291</text:p>
           </table:table-cell>
@@ -7862,7 +7814,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA362</text:p>
           </table:table-cell>
@@ -7892,7 +7844,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH837</text:p>
           </table:table-cell>
@@ -7920,7 +7872,7 @@
               <text:s/>
               2T12345 (10/06/2024 - 15/06/2024), 
               <text:s/>
-              2N1234 (24/06/2024 – 13/07/2024)
+              2N1234 (24/06/2024 - 13/07/2024)
             </text:p>
           </table:table-cell>
           <table:table-cell office:value-type="float" office:value="25" calcext:value-type="float">
@@ -7928,7 +7880,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA370</text:p>
           </table:table-cell>
@@ -7952,7 +7904,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH838</text:p>
           </table:table-cell>
@@ -7976,7 +7928,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro17">
+        <table:table-row table:style-name="ro14">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA369</text:p>
           </table:table-cell>
@@ -8006,7 +7958,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA371</text:p>
           </table:table-cell>
@@ -8030,7 +7982,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA372</text:p>
           </table:table-cell>
@@ -8054,7 +8006,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA379</text:p>
           </table:table-cell>
@@ -8076,7 +8028,7 @@
               <text:s text:c="2"/>
               2N1234 (08/04/2024 - 13/04/2024), 
               <text:s/>
-              2N1234 (29/04/2024 - 11/05/2024), 2N1234 (24/06/2024 – 24/06/2024)
+              2N1234 (29/04/2024 - 11/05/2024), 2N1234 (24/06/2024 - 24/06/2024)
             </text:p>
           </table:table-cell>
           <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
@@ -8084,7 +8036,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA385</text:p>
           </table:table-cell>
@@ -8114,7 +8066,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA384</text:p>
           </table:table-cell>
@@ -8144,7 +8096,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA381</text:p>
           </table:table-cell>
@@ -8176,7 +8128,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA380</text:p>
           </table:table-cell>
@@ -8208,7 +8160,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro18">
+        <table:table-row table:style-name="ro15">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA382</text:p>
           </table:table-cell>
@@ -8232,7 +8184,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA383</text:p>
           </table:table-cell>
@@ -8264,7 +8216,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA386</text:p>
           </table:table-cell>
@@ -8292,7 +8244,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA393</text:p>
           </table:table-cell>
@@ -8309,14 +8261,14 @@
             <text:p>9</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>4N1234 (04/03/2024 - 06/04/2024), 4N1234 (24/06/2024 – 13/07/2024)</text:p>
+            <text:p>4N1234 (04/03/2024 - 06/04/2024), 4N1234 (24/06/2024 - 13/07/2024)</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="float" office:value="40" calcext:value-type="float">
             <text:p>40</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro19">
+        <table:table-row table:style-name="ro16">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA396</text:p>
           </table:table-cell>
@@ -8340,7 +8292,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA394</text:p>
           </table:table-cell>
@@ -8364,7 +8316,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA397</text:p>
           </table:table-cell>
@@ -8392,7 +8344,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA395</text:p>
           </table:table-cell>
@@ -8424,7 +8376,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX997</text:p>
           </table:table-cell>
@@ -8448,7 +8400,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX508</text:p>
           </table:table-cell>
@@ -8476,7 +8428,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH292</text:p>
           </table:table-cell>
@@ -8500,7 +8452,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX966</text:p>
           </table:table-cell>
@@ -8528,7 +8480,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX213</text:p>
           </table:table-cell>
@@ -8552,7 +8504,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA104</text:p>
           </table:table-cell>
@@ -8576,7 +8528,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX969</text:p>
           </table:table-cell>
@@ -8604,7 +8556,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX968</text:p>
           </table:table-cell>
@@ -8632,7 +8584,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH839</text:p>
           </table:table-cell>
@@ -8656,7 +8608,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX503</text:p>
           </table:table-cell>
@@ -8684,7 +8636,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX967</text:p>
           </table:table-cell>
@@ -8712,7 +8664,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX982</text:p>
           </table:table-cell>
@@ -8740,7 +8692,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX981</text:p>
           </table:table-cell>
@@ -8770,7 +8722,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH833</text:p>
           </table:table-cell>
@@ -8794,7 +8746,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX980</text:p>
           </table:table-cell>
@@ -8824,7 +8776,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX983</text:p>
           </table:table-cell>
@@ -8852,7 +8804,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX988</text:p>
           </table:table-cell>
@@ -8876,7 +8828,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX987</text:p>
           </table:table-cell>
@@ -8904,7 +8856,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro20">
+        <table:table-row table:style-name="ro17">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX986</text:p>
           </table:table-cell>
@@ -8970,7 +8922,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX516</text:p>
           </table:table-cell>
@@ -8994,7 +8946,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA213</text:p>
           </table:table-cell>
@@ -9058,7 +9010,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro22">
+        <table:table-row table:style-name="ro18">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX995</text:p>
           </table:table-cell>
@@ -9128,7 +9080,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro23">
+        <table:table-row table:style-name="ro19">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX996</text:p>
           </table:table-cell>
@@ -9170,7 +9122,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS238</text:p>
           </table:table-cell>
@@ -9194,7 +9146,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX529</text:p>
           </table:table-cell>
@@ -9218,7 +9170,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA0374</text:p>
           </table:table-cell>
@@ -9242,7 +9194,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH641</text:p>
           </table:table-cell>
@@ -9266,7 +9218,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA0375</text:p>
           </table:table-cell>
@@ -9290,7 +9242,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA0378</text:p>
           </table:table-cell>
@@ -9314,7 +9266,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA0373</text:p>
           </table:table-cell>
@@ -9338,7 +9290,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA0376</text:p>
           </table:table-cell>
@@ -9362,7 +9314,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA202</text:p>
           </table:table-cell>
@@ -9386,7 +9338,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA0377</text:p>
           </table:table-cell>
@@ -9416,7 +9368,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA175</text:p>
           </table:table-cell>
@@ -9440,7 +9392,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA175</text:p>
           </table:table-cell>
@@ -9464,7 +9416,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro23">
+        <table:table-row table:style-name="ro19">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA179</text:p>
           </table:table-cell>
@@ -9488,7 +9440,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX210</text:p>
           </table:table-cell>
@@ -9512,7 +9464,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH292</text:p>
           </table:table-cell>
@@ -9536,7 +9488,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS238</text:p>
           </table:table-cell>
@@ -9560,7 +9512,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA185</text:p>
           </table:table-cell>
@@ -9584,7 +9536,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA301</text:p>
           </table:table-cell>
@@ -9608,7 +9560,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA181</text:p>
           </table:table-cell>
@@ -9636,7 +9588,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA182</text:p>
           </table:table-cell>
@@ -9660,7 +9612,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA180</text:p>
           </table:table-cell>
@@ -9684,7 +9636,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA282</text:p>
           </table:table-cell>
@@ -9708,7 +9660,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA200</text:p>
           </table:table-cell>
@@ -9732,7 +9684,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA199</text:p>
           </table:table-cell>
@@ -9760,7 +9712,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA201</text:p>
           </table:table-cell>
@@ -9784,7 +9736,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA198</text:p>
           </table:table-cell>
@@ -9812,7 +9764,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA197</text:p>
           </table:table-cell>
@@ -9840,7 +9792,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA196</text:p>
           </table:table-cell>
@@ -9864,7 +9816,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA285</text:p>
           </table:table-cell>
@@ -9896,7 +9848,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro23">
+        <table:table-row table:style-name="ro19">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA286</text:p>
           </table:table-cell>
@@ -9938,7 +9890,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA291</text:p>
           </table:table-cell>
@@ -9966,7 +9918,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA290</text:p>
           </table:table-cell>
@@ -9994,7 +9946,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA298</text:p>
           </table:table-cell>
@@ -10022,7 +9974,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA289</text:p>
           </table:table-cell>
@@ -10046,7 +9998,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro23">
+        <table:table-row table:style-name="ro19">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA292</text:p>
           </table:table-cell>
@@ -10070,7 +10022,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA288</text:p>
           </table:table-cell>
@@ -10094,7 +10046,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA295</text:p>
           </table:table-cell>
@@ -10118,7 +10070,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro23">
+        <table:table-row table:style-name="ro19">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA293</text:p>
           </table:table-cell>
@@ -10142,7 +10094,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA294</text:p>
           </table:table-cell>
@@ -10166,7 +10118,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA297</text:p>
           </table:table-cell>
@@ -10190,7 +10142,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA300</text:p>
           </table:table-cell>
@@ -10214,7 +10166,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA0706</text:p>
           </table:table-cell>
@@ -10238,7 +10190,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA0705</text:p>
           </table:table-cell>
@@ -10262,7 +10214,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA0707</text:p>
           </table:table-cell>
@@ -10286,7 +10238,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1787</text:p>
           </table:table-cell>
@@ -10310,7 +10262,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH521</text:p>
           </table:table-cell>
@@ -10334,7 +10286,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1296</text:p>
           </table:table-cell>
@@ -10358,7 +10310,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1291</text:p>
           </table:table-cell>
@@ -10382,7 +10334,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1289</text:p>
           </table:table-cell>
@@ -10406,7 +10358,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1283</text:p>
           </table:table-cell>
@@ -10430,7 +10382,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH292</text:p>
           </table:table-cell>
@@ -10455,7 +10407,7 @@
           <table:table-cell table:style-name="ce17"/>
           <table:table-cell table:number-columns-repeated="1016"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1035</text:p>
           </table:table-cell>
@@ -10479,7 +10431,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH290</text:p>
           </table:table-cell>
@@ -10503,7 +10455,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1100</text:p>
           </table:table-cell>
@@ -10527,7 +10479,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA104</text:p>
           </table:table-cell>
@@ -10551,7 +10503,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1036</text:p>
           </table:table-cell>
@@ -10575,7 +10527,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS239</text:p>
           </table:table-cell>
@@ -10599,7 +10551,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH839</text:p>
           </table:table-cell>
@@ -10623,7 +10575,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1037</text:p>
           </table:table-cell>
@@ -10647,7 +10599,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH291</text:p>
           </table:table-cell>
@@ -10671,7 +10623,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1038</text:p>
           </table:table-cell>
@@ -10701,7 +10653,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1039</text:p>
           </table:table-cell>
@@ -10733,7 +10685,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH833</text:p>
           </table:table-cell>
@@ -10757,7 +10709,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1087</text:p>
           </table:table-cell>
@@ -10781,7 +10733,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH840</text:p>
           </table:table-cell>
@@ -10805,7 +10757,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1088</text:p>
           </table:table-cell>
@@ -10829,7 +10781,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1099</text:p>
           </table:table-cell>
@@ -10853,7 +10805,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1086</text:p>
           </table:table-cell>
@@ -10877,7 +10829,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1102</text:p>
           </table:table-cell>
@@ -10913,7 +10865,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1104</text:p>
           </table:table-cell>
@@ -10941,7 +10893,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1105</text:p>
           </table:table-cell>
@@ -10969,7 +10921,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH838</text:p>
           </table:table-cell>
@@ -10993,7 +10945,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1103</text:p>
           </table:table-cell>
@@ -11017,7 +10969,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1106</text:p>
           </table:table-cell>
@@ -11051,7 +11003,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1110</text:p>
           </table:table-cell>
@@ -11099,7 +11051,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA237</text:p>
           </table:table-cell>
@@ -11123,7 +11075,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1108</text:p>
           </table:table-cell>
@@ -11147,7 +11099,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1109</text:p>
           </table:table-cell>
@@ -11171,7 +11123,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1107</text:p>
           </table:table-cell>
@@ -11195,7 +11147,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1111</text:p>
           </table:table-cell>
@@ -11219,7 +11171,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1115</text:p>
           </table:table-cell>
@@ -11251,7 +11203,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1112</text:p>
           </table:table-cell>
@@ -11275,7 +11227,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA239</text:p>
           </table:table-cell>
@@ -11337,7 +11289,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA238</text:p>
           </table:table-cell>
@@ -11361,7 +11313,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1114</text:p>
           </table:table-cell>
@@ -11393,7 +11345,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1116</text:p>
           </table:table-cell>
@@ -11427,7 +11379,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1118</text:p>
           </table:table-cell>
@@ -11451,7 +11403,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1119</text:p>
           </table:table-cell>
@@ -11475,7 +11427,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1031</text:p>
           </table:table-cell>
@@ -11523,7 +11475,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA213</text:p>
           </table:table-cell>
@@ -11547,7 +11499,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA240</text:p>
           </table:table-cell>
@@ -11571,7 +11523,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX776</text:p>
           </table:table-cell>
@@ -11595,7 +11547,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1120</text:p>
           </table:table-cell>
@@ -11619,7 +11571,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro24">
+        <table:table-row table:style-name="ro20">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH162</text:p>
           </table:table-cell>
@@ -11643,7 +11595,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1123</text:p>
           </table:table-cell>
@@ -11667,7 +11619,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1124</text:p>
           </table:table-cell>
@@ -11691,7 +11643,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1125</text:p>
           </table:table-cell>
@@ -11799,7 +11751,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro23">
+        <table:table-row table:style-name="ro19">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1121</text:p>
           </table:table-cell>
@@ -11837,7 +11789,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1126</text:p>
           </table:table-cell>
@@ -11871,7 +11823,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1129</text:p>
           </table:table-cell>
@@ -11895,7 +11847,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1280</text:p>
           </table:table-cell>
@@ -11919,7 +11871,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1130</text:p>
           </table:table-cell>
@@ -11973,7 +11925,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1127</text:p>
           </table:table-cell>
@@ -11997,7 +11949,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1131</text:p>
           </table:table-cell>
@@ -12021,7 +11973,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1133</text:p>
           </table:table-cell>
@@ -12045,7 +11997,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS238</text:p>
           </table:table-cell>
@@ -12069,7 +12021,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1132</text:p>
           </table:table-cell>
@@ -12099,7 +12051,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1134</text:p>
           </table:table-cell>
@@ -12131,19 +12083,19 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6" table:number-rows-repeated="1048111">
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="1048111">
           <table:table-cell table:number-columns-repeated="1024"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro1">
           <table:table-cell table:number-columns-repeated="1024"/>
         </table:table-row>
       </table:table>
       <table:table table:name="Turmas Divididas" table:style-name="ta1">
-        <table:table-column table:style-name="co9" table:number-columns-repeated="14" table:default-cell-style-name="ce22"/>
-        <table:table-column table:style-name="co9" table:default-cell-style-name="ce29"/>
-        <table:table-column table:style-name="co9" table:number-columns-repeated="1008" table:default-cell-style-name="ce16"/>
-        <table:table-column table:style-name="co9" table:default-cell-style-name="ce17"/>
-        <table:table-row table:style-name="ro3">
+        <table:table-column table:style-name="co1" table:number-columns-repeated="14" table:default-cell-style-name="ce22"/>
+        <table:table-column table:style-name="co1" table:default-cell-style-name="ce29"/>
+        <table:table-column table:style-name="co1" table:number-columns-repeated="1008" table:default-cell-style-name="ce16"/>
+        <table:table-column table:style-name="co1" table:default-cell-style-name="ce17"/>
+        <table:table-row table:style-name="ro2">
           <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
             <text:p>ano</text:p>
           </table:table-cell>
@@ -12380,7 +12332,7 @@
           <table:covered-table-cell table:style-name="ce22"/>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -12480,7 +12432,7 @@
           <table:covered-table-cell table:style-name="ce22"/>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -12528,7 +12480,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -12574,7 +12526,7 @@
           <table:covered-table-cell table:style-name="ce22"/>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -12622,7 +12574,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -12876,9 +12828,9 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.2">
   <office:meta>
     <meta:generator>LibreOffice/6.4.7.2$Linux_X86_64 LibreOffice_project/40$Build-2</meta:generator>
-    <dc:date>2024-02-27T13:19:01.922582536</dc:date>
-    <meta:editing-duration>PT3H11M31S</meta:editing-duration>
-    <meta:editing-cycles>27</meta:editing-cycles>
+    <dc:date>2024-05-20T16:02:21.267963298</dc:date>
+    <meta:editing-duration>PT3H28M50S</meta:editing-duration>
+    <meta:editing-cycles>31</meta:editing-cycles>
     <meta:document-statistic meta:table-count="2" meta:cell-count="3466" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
@@ -12890,8 +12842,8 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">50270</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">307191</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">84652</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">306840</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
@@ -12916,7 +12868,7 @@
             </config:config-item-map-entry>
             <config:config-item-map-entry config:name="_WITH_docentes_por_turma_AS_SELECT_dt_id_turma_COALESCE_COUNT_p__202402211025">
               <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">284</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -12925,7 +12877,7 @@
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">263</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">95</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -12934,7 +12886,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">_WITH_docentes_por_turma_AS_SELECT_dt_id_turma_COALESCE_COUNT_p__202402211025</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1307</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1861</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">95</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -12971,7 +12923,7 @@
       <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
       <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">lAH+/0Rlc2tKZXQtMjYwMAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAQ1VQUzpEZXNrSmV0LTI2MDAAAAAAAAAAAAAAAAAAAAAWAAMAsQAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9RGVza0pldC0yNjAwCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luZGFqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4RGF0YQpQYWdlU2l6ZTpBNAAAEgBDT01QQVRfRFVQTEVYX01PREUTAER1cGxleE1vZGU6OlVua25vd24=</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">kwH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAtAAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luZGFqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4RGF0YQpQYWdlU2l6ZTpBNAAAEgBDT01QQVRfRFVQTEVYX01PREUPAER1cGxleE1vZGU6Ok9mZg==</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1000</config:config-item>
       <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
@@ -12993,7 +12945,7 @@
       <config:config-item config:name="EmbedFonts" config:type="boolean">false</config:config-item>
       <config:config-item config:name="SaveThumbnail" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string">DeskJet-2600</config:config-item>
+      <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
       <config:config-item config:name="CharacterCompressionType" config:type="short">0</config:config-item>
       <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
@@ -13025,8 +12977,8 @@
       <number:number number:min-integer-digits="1"/>
     </number:number-style>
     <style:style style:name="Default" style:family="table-cell"/>
-    <style:style style:name="Heading" style:family="table-cell" style:parent-style-name="Default">
-      <style:text-properties fo:color="#000000" fo:font-size="24pt" fo:font-style="normal" fo:font-weight="bold" style:font-size-asian="24pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-size-complex="24pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
+    <style:style style:name="Heading_20__28_user_29_" style:display-name="Heading (user)" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties fo:color="#000000" fo:font-size="24pt" fo:font-style="normal" fo:font-weight="bold"/>
     </style:style>
     <style:style style:name="Heading_20_1" style:display-name="Heading 1" style:family="table-cell" style:parent-style-name="Heading">
       <style:text-properties fo:font-size="18pt" style:font-size-asian="18pt" style:font-size-complex="18pt"/>
@@ -13079,6 +13031,12 @@
     <style:style style:name="Accent_20_3" style:display-name="Accent 3" style:family="table-cell" style:parent-style-name="Accent">
       <style:table-cell-properties fo:background-color="#dddddd"/>
     </style:style>
+    <style:style style:name="Result_20__28_user_29_" style:display-name="Result (user)" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties fo:color="#000000" fo:font-size="10pt" fo:font-style="italic" style:text-underline-style="solid" style:text-underline-width="auto" style:text-underline-color="#000000" fo:font-weight="bold"/>
+    </style:style>
+    <style:style style:name="Heading" style:family="table-cell" style:parent-style-name="Default">
+      <style:text-properties fo:color="#000000" fo:font-size="24pt" fo:font-style="normal" fo:font-weight="bold" style:font-size-asian="24pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-size-complex="24pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
+    </style:style>
     <style:style style:name="Result" style:family="table-cell" style:parent-style-name="Default">
       <style:text-properties fo:font-style="italic" style:text-underline-style="solid" style:text-underline-width="auto" style:text-underline-color="font-color" fo:font-weight="bold" style:font-style-asian="italic" style:font-weight-asian="bold" style:font-style-complex="italic" style:font-weight-complex="bold"/>
     </style:style>
@@ -13127,9 +13085,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2024-02-27">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2024-05-20">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="13:19:06.881938970">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="15:45:00.242002512">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>